<commit_message>
add multi-camera processing function
</commit_message>
<xml_diff>
--- a/Cam1calib.xlsx
+++ b/Cam1calib.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB44A5F8-6773-4CD2-A730-E4947A80C96C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C94347-66B9-404C-993F-408BEABE2933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="3489" windowWidth="24686" windowHeight="13217" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14769" yWindow="3531" windowWidth="24685" windowHeight="13218" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -345,20 +345,20 @@
   <dimension ref="A1:E420"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D90"/>
+      <selection sqref="A1:D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
-        <v>900.95100000000002</v>
+        <v>906.98199999999997</v>
       </c>
       <c r="B1" s="1">
-        <v>1031.3440000000001</v>
+        <v>1030.79</v>
       </c>
       <c r="C1" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D1" s="1">
         <v>0</v>
@@ -367,253 +367,253 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>920.04200000000003</v>
+        <v>929.92399999999998</v>
       </c>
       <c r="B2" s="1">
-        <v>1793.712</v>
+        <v>1819.107</v>
       </c>
       <c r="C2" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D2" s="1">
-        <v>-16.079999999999998</v>
+        <v>-15.92</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>915.75599999999997</v>
+        <v>924.78899999999999</v>
       </c>
       <c r="B3" s="1">
-        <v>1688.8820000000001</v>
+        <v>1723.2149999999999</v>
       </c>
       <c r="C3" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D3" s="1">
-        <v>-13.98</v>
+        <v>-14.02</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>911.81</v>
+        <v>920.03200000000004</v>
       </c>
       <c r="B4" s="1">
-        <v>1590.5</v>
+        <v>1621.116</v>
       </c>
       <c r="C4" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D4" s="1">
-        <v>-11.98</v>
+        <v>-12</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>908.33</v>
+        <v>916.02599999999995</v>
       </c>
       <c r="B5" s="1">
-        <v>1494.0050000000001</v>
+        <v>1522.23</v>
       </c>
       <c r="C5" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D5" s="1">
-        <v>-9.98</v>
+        <v>-10</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>905.35799999999995</v>
+        <v>912.98699999999997</v>
       </c>
       <c r="B6" s="1">
-        <v>1397.7670000000001</v>
+        <v>1425.0650000000001</v>
       </c>
       <c r="C6" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D6" s="1">
-        <v>-8</v>
+        <v>-8.02</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>903.71699999999998</v>
+        <v>910.43700000000001</v>
       </c>
       <c r="B7" s="1">
-        <v>1300.5250000000001</v>
+        <v>1327.85</v>
       </c>
       <c r="C7" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D7" s="1">
-        <v>-6</v>
+        <v>-6.05</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>901.79</v>
+        <v>908.55</v>
       </c>
       <c r="B8" s="1">
-        <v>1205.059</v>
+        <v>1228.954</v>
       </c>
       <c r="C8" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D8" s="1">
-        <v>-4</v>
+        <v>-4.05</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>900.70399999999995</v>
+        <v>907.07100000000003</v>
       </c>
       <c r="B9" s="1">
-        <v>1109.7550000000001</v>
+        <v>1131.1769999999999</v>
       </c>
       <c r="C9" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D9" s="1">
-        <v>-2</v>
+        <v>-2.0499999999999998</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>900.85400000000004</v>
+        <v>906.98199999999997</v>
       </c>
       <c r="B10" s="1">
-        <v>1015.58</v>
+        <v>1033.8689999999999</v>
       </c>
       <c r="C10" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>903.08600000000001</v>
+        <v>906.995</v>
       </c>
       <c r="B11" s="1">
-        <v>920.33500000000004</v>
+        <v>935.88300000000004</v>
       </c>
       <c r="C11" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D11" s="1">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>905.38599999999997</v>
+        <v>908</v>
       </c>
       <c r="B12" s="1">
-        <v>824.85900000000004</v>
+        <v>838.10799999999995</v>
       </c>
       <c r="C12" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D12" s="1">
-        <v>4</v>
+        <v>3.95</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>908.27700000000004</v>
+        <v>909.577</v>
       </c>
       <c r="B13" s="1">
-        <v>728.41399999999999</v>
+        <v>740.32100000000003</v>
       </c>
       <c r="C13" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D13" s="1">
-        <v>5.97</v>
+        <v>5.92</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>911.4</v>
+        <v>911.99900000000002</v>
       </c>
       <c r="B14" s="1">
-        <v>630.721</v>
+        <v>640.15800000000002</v>
       </c>
       <c r="C14" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D14" s="1">
-        <v>8.02</v>
+        <v>7.95</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>915.572</v>
+        <v>915.36500000000001</v>
       </c>
       <c r="B15" s="1">
-        <v>535.27099999999996</v>
+        <v>540.43700000000001</v>
       </c>
       <c r="C15" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D15" s="1">
-        <v>10.02</v>
+        <v>9.98</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>920.39300000000003</v>
+        <v>918.95799999999997</v>
       </c>
       <c r="B16" s="1">
-        <v>438.435</v>
+        <v>440.56400000000002</v>
       </c>
       <c r="C16" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D16" s="1">
-        <v>12.02</v>
+        <v>11.98</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>925.78800000000001</v>
+        <v>923.43700000000001</v>
       </c>
       <c r="B17" s="1">
-        <v>338.82499999999999</v>
+        <v>340.76100000000002</v>
       </c>
       <c r="C17" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D17" s="1">
-        <v>14.02</v>
+        <v>14</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>933.97400000000005</v>
+        <v>928.48900000000003</v>
       </c>
       <c r="B18" s="1">
-        <v>239.63</v>
+        <v>238.92099999999999</v>
       </c>
       <c r="C18" s="1">
-        <v>2553.1999999999998</v>
+        <v>2501.1</v>
       </c>
       <c r="D18" s="1">
         <v>16</v>
@@ -622,13 +622,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>883.154</v>
+        <v>887.98599999999999</v>
       </c>
       <c r="B19" s="1">
-        <v>1031.001</v>
+        <v>1031.145</v>
       </c>
       <c r="C19" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -637,58 +637,58 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>901.95</v>
+        <v>910.25900000000001</v>
       </c>
       <c r="B20" s="1">
-        <v>1809.098</v>
+        <v>1818.2239999999999</v>
       </c>
       <c r="C20" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D20" s="1">
-        <v>-16.100000000000001</v>
+        <v>-15.92</v>
       </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>897.87</v>
+        <v>905.36300000000006</v>
       </c>
       <c r="B21" s="1">
-        <v>1703.0340000000001</v>
+        <v>1721.8820000000001</v>
       </c>
       <c r="C21" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D21" s="1">
-        <v>-14</v>
+        <v>-14.02</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>893.97500000000002</v>
+        <v>900.87099999999998</v>
       </c>
       <c r="B22" s="1">
-        <v>1603.57</v>
+        <v>1620.346</v>
       </c>
       <c r="C22" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D22" s="1">
-        <v>-11.95</v>
+        <v>-12</v>
       </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>890.61500000000001</v>
+        <v>897.00599999999997</v>
       </c>
       <c r="B23" s="1">
-        <v>1508.3330000000001</v>
+        <v>1522.2370000000001</v>
       </c>
       <c r="C23" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D23" s="1">
         <v>-10</v>
@@ -697,43 +697,43 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>887.70600000000002</v>
+        <v>893.98599999999999</v>
       </c>
       <c r="B24" s="1">
-        <v>1410.9469999999999</v>
+        <v>1424.569</v>
       </c>
       <c r="C24" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D24" s="1">
-        <v>-7.97</v>
+        <v>-8.02</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>885.99800000000005</v>
+        <v>891.38099999999997</v>
       </c>
       <c r="B25" s="1">
-        <v>1315.5519999999999</v>
+        <v>1327.3340000000001</v>
       </c>
       <c r="C25" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D25" s="1">
-        <v>-6</v>
+        <v>-6.05</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>884.60400000000004</v>
+        <v>889.68399999999997</v>
       </c>
       <c r="B26" s="1">
-        <v>1219.835</v>
+        <v>1228.8389999999999</v>
       </c>
       <c r="C26" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D26" s="1">
         <v>-4.0199999999999996</v>
@@ -742,163 +742,163 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>882.74099999999999</v>
+        <v>888.23299999999995</v>
       </c>
       <c r="B27" s="1">
-        <v>1123.1389999999999</v>
+        <v>1132.3530000000001</v>
       </c>
       <c r="C27" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D27" s="1">
-        <v>-2</v>
+        <v>-2.08</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>883.08799999999997</v>
+        <v>887.98099999999999</v>
       </c>
       <c r="B28" s="1">
-        <v>1028.4639999999999</v>
+        <v>1033.259</v>
       </c>
       <c r="C28" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D28" s="1">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>884.89300000000003</v>
+        <v>888.00599999999997</v>
       </c>
       <c r="B29" s="1">
-        <v>935.43399999999997</v>
+        <v>935.69100000000003</v>
       </c>
       <c r="C29" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D29" s="1">
-        <v>2</v>
+        <v>1.98</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>887.22199999999998</v>
+        <v>889</v>
       </c>
       <c r="B30" s="1">
-        <v>840.12800000000004</v>
+        <v>839.68100000000004</v>
       </c>
       <c r="C30" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D30" s="1">
-        <v>3.98</v>
+        <v>3.92</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>890.13699999999994</v>
+        <v>890.70500000000004</v>
       </c>
       <c r="B31" s="1">
-        <v>742.30399999999997</v>
+        <v>740.41200000000003</v>
       </c>
       <c r="C31" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D31" s="1">
-        <v>5.98</v>
+        <v>5.95</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>893.21100000000001</v>
+        <v>893.00800000000004</v>
       </c>
       <c r="B32" s="1">
-        <v>646.08000000000004</v>
+        <v>641.89499999999998</v>
       </c>
       <c r="C32" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D32" s="1">
-        <v>8.0299999999999994</v>
+        <v>7.92</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>896.77700000000004</v>
+        <v>895.92600000000004</v>
       </c>
       <c r="B33" s="1">
-        <v>550.12599999999998</v>
+        <v>540.91999999999996</v>
       </c>
       <c r="C33" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D33" s="1">
-        <v>10.029999999999999</v>
+        <v>10</v>
       </c>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>901.423</v>
+        <v>899.60900000000004</v>
       </c>
       <c r="B34" s="1">
-        <v>453.45800000000003</v>
+        <v>442.29899999999998</v>
       </c>
       <c r="C34" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D34" s="1">
-        <v>12.03</v>
+        <v>11.98</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>906.61199999999997</v>
+        <v>903.83299999999997</v>
       </c>
       <c r="B35" s="1">
-        <v>355.49299999999999</v>
+        <v>342.43</v>
       </c>
       <c r="C35" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D35" s="1">
-        <v>14.03</v>
+        <v>14</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>913.27200000000005</v>
+        <v>908.67200000000003</v>
       </c>
       <c r="B36" s="1">
-        <v>255.81399999999999</v>
+        <v>240.833</v>
       </c>
       <c r="C36" s="1">
-        <v>2652.9</v>
+        <v>2600.8000000000002</v>
       </c>
       <c r="D36" s="1">
-        <v>16</v>
+        <v>15.98</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>866.351</v>
+        <v>870.35</v>
       </c>
       <c r="B37" s="1">
-        <v>1030.9739999999999</v>
+        <v>1031.203</v>
       </c>
       <c r="C37" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -907,103 +907,103 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>884.46400000000006</v>
+        <v>892.09900000000005</v>
       </c>
       <c r="B38" s="1">
-        <v>1808.2180000000001</v>
+        <v>1817.807</v>
       </c>
       <c r="C38" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D38" s="1">
-        <v>-16.100000000000001</v>
+        <v>-15.92</v>
       </c>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>880.65499999999997</v>
+        <v>887.33500000000004</v>
       </c>
       <c r="B39" s="1">
-        <v>1701.82</v>
+        <v>1721.537</v>
       </c>
       <c r="C39" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D39" s="1">
-        <v>-14</v>
+        <v>-14.02</v>
       </c>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>876.76199999999994</v>
+        <v>882.971</v>
       </c>
       <c r="B40" s="1">
-        <v>1602.326</v>
+        <v>1620.2560000000001</v>
       </c>
       <c r="C40" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D40" s="1">
-        <v>-11.95</v>
+        <v>-11.97</v>
       </c>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>873.74599999999998</v>
+        <v>879.11400000000003</v>
       </c>
       <c r="B41" s="1">
-        <v>1506.9570000000001</v>
+        <v>1523.125</v>
       </c>
       <c r="C41" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D41" s="1">
-        <v>-10</v>
+        <v>-10.02</v>
       </c>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>871.08399999999995</v>
+        <v>876.14099999999996</v>
       </c>
       <c r="B42" s="1">
-        <v>1410.5840000000001</v>
+        <v>1424.558</v>
       </c>
       <c r="C42" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D42" s="1">
-        <v>-7.97</v>
+        <v>-8.02</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>869.29600000000005</v>
+        <v>873.94500000000005</v>
       </c>
       <c r="B43" s="1">
-        <v>1315.164</v>
+        <v>1327.33</v>
       </c>
       <c r="C43" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D43" s="1">
-        <v>-6</v>
+        <v>-6.05</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>867.98699999999997</v>
+        <v>872.00800000000004</v>
       </c>
       <c r="B44" s="1">
-        <v>1220.163</v>
+        <v>1228.9870000000001</v>
       </c>
       <c r="C44" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D44" s="1">
         <v>-4.0199999999999996</v>
@@ -1012,163 +1012,163 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>866.43299999999999</v>
+        <v>870.96699999999998</v>
       </c>
       <c r="B45" s="1">
-        <v>1123.518</v>
+        <v>1132.9949999999999</v>
       </c>
       <c r="C45" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D45" s="1">
-        <v>-2</v>
+        <v>-2.08</v>
       </c>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>866.32500000000005</v>
+        <v>870.36500000000001</v>
       </c>
       <c r="B46" s="1">
-        <v>1028.0170000000001</v>
+        <v>1033.9469999999999</v>
       </c>
       <c r="C46" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D46" s="1">
-        <v>0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>868.24800000000005</v>
+        <v>870.75699999999995</v>
       </c>
       <c r="B47" s="1">
-        <v>935.73800000000006</v>
+        <v>936.274</v>
       </c>
       <c r="C47" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D47" s="1">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>870.87699999999995</v>
+        <v>871.61199999999997</v>
       </c>
       <c r="B48" s="1">
-        <v>840.49300000000005</v>
+        <v>839.01499999999999</v>
       </c>
       <c r="C48" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D48" s="1">
-        <v>3.98</v>
+        <v>3.95</v>
       </c>
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
-        <v>873.56100000000004</v>
+        <v>873</v>
       </c>
       <c r="B49" s="1">
-        <v>743.47400000000005</v>
+        <v>741.32399999999996</v>
       </c>
       <c r="C49" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D49" s="1">
-        <v>5.98</v>
+        <v>5.92</v>
       </c>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
-        <v>876.40099999999995</v>
+        <v>875.28300000000002</v>
       </c>
       <c r="B50" s="1">
-        <v>645.774</v>
+        <v>641.37699999999995</v>
       </c>
       <c r="C50" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D50" s="1">
-        <v>8.0299999999999994</v>
+        <v>7.95</v>
       </c>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
-        <v>880.17399999999998</v>
+        <v>878.45100000000002</v>
       </c>
       <c r="B51" s="1">
-        <v>550.495</v>
+        <v>541.90700000000004</v>
       </c>
       <c r="C51" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D51" s="1">
-        <v>10.029999999999999</v>
+        <v>9.98</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
-        <v>884.53499999999997</v>
+        <v>881.66099999999994</v>
       </c>
       <c r="B52" s="1">
-        <v>453.92599999999999</v>
+        <v>443.20100000000002</v>
       </c>
       <c r="C52" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D52" s="1">
-        <v>12.03</v>
+        <v>12</v>
       </c>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
-        <v>889.59299999999996</v>
+        <v>885.83</v>
       </c>
       <c r="B53" s="1">
-        <v>356.06299999999999</v>
+        <v>343.63499999999999</v>
       </c>
       <c r="C53" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D53" s="1">
-        <v>14.03</v>
+        <v>14</v>
       </c>
       <c r="E53" s="1"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
-        <v>895.92100000000005</v>
+        <v>890.50699999999995</v>
       </c>
       <c r="B54" s="1">
-        <v>256.73</v>
+        <v>242.49100000000001</v>
       </c>
       <c r="C54" s="1">
-        <v>2752.6</v>
+        <v>2700.5</v>
       </c>
       <c r="D54" s="1">
-        <v>16</v>
+        <v>15.98</v>
       </c>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
-        <v>851.13099999999997</v>
+        <v>854.11099999999999</v>
       </c>
       <c r="B55" s="1">
-        <v>1030.8420000000001</v>
+        <v>1031.172</v>
       </c>
       <c r="C55" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -1177,43 +1177,43 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
-        <v>868.44799999999998</v>
+        <v>875.20299999999997</v>
       </c>
       <c r="B56" s="1">
-        <v>1806.579</v>
+        <v>1816.9449999999999</v>
       </c>
       <c r="C56" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D56" s="1">
-        <v>-16.100000000000001</v>
+        <v>-15.92</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
-        <v>864.69799999999998</v>
+        <v>870.66399999999999</v>
       </c>
       <c r="B57" s="1">
-        <v>1700.71</v>
+        <v>1720.9680000000001</v>
       </c>
       <c r="C57" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D57" s="1">
-        <v>-13.97</v>
+        <v>-14.02</v>
       </c>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>861.29</v>
+        <v>866.30100000000004</v>
       </c>
       <c r="B58" s="1">
-        <v>1603.29</v>
+        <v>1619.6320000000001</v>
       </c>
       <c r="C58" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D58" s="1">
         <v>-11.97</v>
@@ -1222,223 +1222,223 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
-        <v>858.20600000000002</v>
+        <v>862.96400000000006</v>
       </c>
       <c r="B59" s="1">
-        <v>1506.614</v>
+        <v>1522.2190000000001</v>
       </c>
       <c r="C59" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D59" s="1">
-        <v>-10</v>
+        <v>-10.02</v>
       </c>
       <c r="E59" s="1"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
-        <v>855.48</v>
+        <v>859.94899999999996</v>
       </c>
       <c r="B60" s="1">
-        <v>1409.741</v>
+        <v>1424.5029999999999</v>
       </c>
       <c r="C60" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D60" s="1">
-        <v>-7.97</v>
+        <v>-8.02</v>
       </c>
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
-        <v>853.702</v>
+        <v>857.46</v>
       </c>
       <c r="B61" s="1">
-        <v>1315.0930000000001</v>
+        <v>1327.046</v>
       </c>
       <c r="C61" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D61" s="1">
-        <v>-6</v>
+        <v>-6.05</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
-        <v>852.53099999999995</v>
+        <v>855.846</v>
       </c>
       <c r="B62" s="1">
-        <v>1219.47</v>
+        <v>1228.8579999999999</v>
       </c>
       <c r="C62" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D62" s="1">
-        <v>-4</v>
+        <v>-4.0199999999999996</v>
       </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
-        <v>850.99</v>
+        <v>854.88</v>
       </c>
       <c r="B63" s="1">
-        <v>1124.3620000000001</v>
+        <v>1132.915</v>
       </c>
       <c r="C63" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D63" s="1">
-        <v>-2</v>
+        <v>-2.08</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
-        <v>851.09</v>
+        <v>854.10199999999998</v>
       </c>
       <c r="B64" s="1">
-        <v>1030.432</v>
+        <v>1033.8910000000001</v>
       </c>
       <c r="C64" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D64" s="1">
-        <v>0</v>
+        <v>-0.02</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
-        <v>852.89400000000001</v>
+        <v>854.36599999999999</v>
       </c>
       <c r="B65" s="1">
-        <v>936.39099999999996</v>
+        <v>938.4</v>
       </c>
       <c r="C65" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D65" s="1">
-        <v>2</v>
+        <v>1.92</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
-        <v>855.30799999999999</v>
+        <v>855.03099999999995</v>
       </c>
       <c r="B66" s="1">
-        <v>841.17399999999998</v>
+        <v>839.59</v>
       </c>
       <c r="C66" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D66" s="1">
-        <v>3.98</v>
+        <v>3.95</v>
       </c>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
-        <v>858.13800000000003</v>
+        <v>856.91300000000001</v>
       </c>
       <c r="B67" s="1">
-        <v>744.08199999999999</v>
+        <v>741.37599999999998</v>
       </c>
       <c r="C67" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D67" s="1">
-        <v>5.98</v>
+        <v>5.95</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
-        <v>860.78899999999999</v>
+        <v>858.97</v>
       </c>
       <c r="B68" s="1">
-        <v>646.63499999999999</v>
+        <v>643.40499999999997</v>
       </c>
       <c r="C68" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D68" s="1">
-        <v>8</v>
+        <v>7.92</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>864.53099999999995</v>
+        <v>861.65499999999997</v>
       </c>
       <c r="B69" s="1">
-        <v>550.45299999999997</v>
+        <v>542.47500000000002</v>
       </c>
       <c r="C69" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D69" s="1">
-        <v>10.050000000000001</v>
+        <v>10</v>
       </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>868.62300000000005</v>
+        <v>865.197</v>
       </c>
       <c r="B70" s="1">
-        <v>455.084</v>
+        <v>445.267</v>
       </c>
       <c r="C70" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D70" s="1">
-        <v>12.03</v>
+        <v>11.98</v>
       </c>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>873.61300000000006</v>
+        <v>869.10199999999998</v>
       </c>
       <c r="B71" s="1">
-        <v>358.00700000000001</v>
+        <v>344.17899999999997</v>
       </c>
       <c r="C71" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D71" s="1">
-        <v>14.03</v>
+        <v>14</v>
       </c>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>879.98699999999997</v>
+        <v>873.54300000000001</v>
       </c>
       <c r="B72" s="1">
-        <v>257.065</v>
+        <v>243.15</v>
       </c>
       <c r="C72" s="1">
-        <v>2852.3</v>
+        <v>2800.2</v>
       </c>
       <c r="D72" s="1">
-        <v>16</v>
+        <v>15.98</v>
       </c>
       <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
-        <v>837.02800000000002</v>
+        <v>839.06299999999999</v>
       </c>
       <c r="B73" s="1">
-        <v>1031.298</v>
+        <v>1031.307</v>
       </c>
       <c r="C73" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
@@ -1447,58 +1447,58 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
-        <v>853.39400000000001</v>
+        <v>859.47</v>
       </c>
       <c r="B74" s="1">
-        <v>1806.33</v>
+        <v>1816.1849999999999</v>
       </c>
       <c r="C74" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D74" s="1">
-        <v>-16.100000000000001</v>
+        <v>-15.92</v>
       </c>
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
-        <v>849.88599999999997</v>
+        <v>855.15700000000004</v>
       </c>
       <c r="B75" s="1">
-        <v>1700.5050000000001</v>
+        <v>1720.5029999999999</v>
       </c>
       <c r="C75" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D75" s="1">
-        <v>-14</v>
+        <v>-14.02</v>
       </c>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
-        <v>846.61699999999996</v>
+        <v>850.97799999999995</v>
       </c>
       <c r="B76" s="1">
-        <v>1601.857</v>
+        <v>1619.78</v>
       </c>
       <c r="C76" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D76" s="1">
-        <v>-11.95</v>
+        <v>-12</v>
       </c>
       <c r="E76" s="1"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
-        <v>843.59799999999996</v>
+        <v>847.44</v>
       </c>
       <c r="B77" s="1">
-        <v>1506.2180000000001</v>
+        <v>1521.47</v>
       </c>
       <c r="C77" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D77" s="1">
         <v>-10</v>
@@ -1507,43 +1507,43 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
-        <v>841.14599999999996</v>
+        <v>844.77499999999998</v>
       </c>
       <c r="B78" s="1">
-        <v>1409.758</v>
+        <v>1424.191</v>
       </c>
       <c r="C78" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D78" s="1">
-        <v>-7.97</v>
+        <v>-8.02</v>
       </c>
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
-        <v>839.43100000000004</v>
+        <v>842.38699999999994</v>
       </c>
       <c r="B79" s="1">
-        <v>1315.2729999999999</v>
+        <v>1327.441</v>
       </c>
       <c r="C79" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D79" s="1">
-        <v>-6</v>
+        <v>-6.05</v>
       </c>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
-        <v>838.43100000000004</v>
+        <v>840.58</v>
       </c>
       <c r="B80" s="1">
-        <v>1219.684</v>
+        <v>1229.2750000000001</v>
       </c>
       <c r="C80" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D80" s="1">
         <v>-4.0199999999999996</v>
@@ -1552,278 +1552,422 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
-        <v>836.96699999999998</v>
+        <v>839.62</v>
       </c>
       <c r="B81" s="1">
-        <v>1123.827</v>
+        <v>1132.7070000000001</v>
       </c>
       <c r="C81" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D81" s="1">
-        <v>-2</v>
+        <v>-2.08</v>
       </c>
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
-        <v>837.12400000000002</v>
+        <v>839.09699999999998</v>
       </c>
       <c r="B82" s="1">
-        <v>1030.2339999999999</v>
+        <v>1034.557</v>
       </c>
       <c r="C82" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D82" s="1">
-        <v>0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
-        <v>838.70100000000002</v>
+        <v>839.20899999999995</v>
       </c>
       <c r="B83" s="1">
-        <v>937.24699999999996</v>
+        <v>938.78099999999995</v>
       </c>
       <c r="C83" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D83" s="1">
-        <v>1.98</v>
+        <v>1.92</v>
       </c>
       <c r="E83" s="1"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
-        <v>841.20699999999999</v>
+        <v>840.029</v>
       </c>
       <c r="B84" s="1">
-        <v>840.52</v>
+        <v>839.51400000000001</v>
       </c>
       <c r="C84" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D84" s="1">
-        <v>3.98</v>
+        <v>3.95</v>
       </c>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
-        <v>843.59</v>
+        <v>841.78399999999999</v>
       </c>
       <c r="B85" s="1">
-        <v>744.41200000000003</v>
+        <v>741.76400000000001</v>
       </c>
       <c r="C85" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D85" s="1">
-        <v>6</v>
+        <v>5.92</v>
       </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
-        <v>846.46500000000003</v>
+        <v>843.88499999999999</v>
       </c>
       <c r="B86" s="1">
-        <v>648.22299999999996</v>
+        <v>642.73299999999995</v>
       </c>
       <c r="C86" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D86" s="1">
-        <v>8</v>
+        <v>7.95</v>
       </c>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
-        <v>849.7</v>
+        <v>846.49099999999999</v>
       </c>
       <c r="B87" s="1">
-        <v>551.73599999999999</v>
+        <v>543.30200000000002</v>
       </c>
       <c r="C87" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D87" s="1">
-        <v>10.050000000000001</v>
+        <v>10</v>
       </c>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
-        <v>853.76300000000003</v>
+        <v>849.55799999999999</v>
       </c>
       <c r="B88" s="1">
-        <v>456.90600000000001</v>
+        <v>445.72300000000001</v>
       </c>
       <c r="C88" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D88" s="1">
-        <v>12</v>
+        <v>11.98</v>
       </c>
       <c r="E88" s="1"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
-        <v>858.71699999999998</v>
+        <v>853.66499999999996</v>
       </c>
       <c r="B89" s="1">
-        <v>358.25900000000001</v>
+        <v>345.22300000000001</v>
       </c>
       <c r="C89" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D89" s="1">
-        <v>14.03</v>
+        <v>14</v>
       </c>
       <c r="E89" s="1"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
-        <v>865.05799999999999</v>
+        <v>857.84500000000003</v>
       </c>
       <c r="B90" s="1">
-        <v>256.779</v>
+        <v>244.85400000000001</v>
       </c>
       <c r="C90" s="1">
-        <v>2952</v>
+        <v>2899.9</v>
       </c>
       <c r="D90" s="1">
-        <v>16.03</v>
+        <v>15.98</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
+      <c r="A91" s="1">
+        <v>825.17700000000002</v>
+      </c>
+      <c r="B91" s="1">
+        <v>1030.8030000000001</v>
+      </c>
+      <c r="C91" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D91" s="1">
+        <v>0</v>
+      </c>
       <c r="E91" s="1"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
+      <c r="A92" s="1">
+        <v>844.846</v>
+      </c>
+      <c r="B92" s="1">
+        <v>1816.2629999999999</v>
+      </c>
+      <c r="C92" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D92" s="1">
+        <v>-15.9</v>
+      </c>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
+      <c r="A93" s="1">
+        <v>840.45799999999997</v>
+      </c>
+      <c r="B93" s="1">
+        <v>1717.9829999999999</v>
+      </c>
+      <c r="C93" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D93" s="1">
+        <v>-14.03</v>
+      </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
+      <c r="A94" s="1">
+        <v>836.56399999999996</v>
+      </c>
+      <c r="B94" s="1">
+        <v>1617.6849999999999</v>
+      </c>
+      <c r="C94" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D94" s="1">
+        <v>-11.98</v>
+      </c>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
+      <c r="A95" s="1">
+        <v>833.11500000000001</v>
+      </c>
+      <c r="B95" s="1">
+        <v>1520.3209999999999</v>
+      </c>
+      <c r="C95" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D95" s="1">
+        <v>-10.029999999999999</v>
+      </c>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
+      <c r="A96" s="1">
+        <v>830.33</v>
+      </c>
+      <c r="B96" s="1">
+        <v>1422.3130000000001</v>
+      </c>
+      <c r="C96" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D96" s="1">
+        <v>-8.0299999999999994</v>
+      </c>
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
+      <c r="A97" s="1">
+        <v>828.125</v>
+      </c>
+      <c r="B97" s="1">
+        <v>1324.91</v>
+      </c>
+      <c r="C97" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D97" s="1">
+        <v>-6.03</v>
+      </c>
       <c r="E97" s="1"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
+      <c r="A98" s="1">
+        <v>826.50599999999997</v>
+      </c>
+      <c r="B98" s="1">
+        <v>1228.5609999999999</v>
+      </c>
+      <c r="C98" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D98" s="1">
+        <v>-4.05</v>
+      </c>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
+      <c r="A99" s="1">
+        <v>825.59</v>
+      </c>
+      <c r="B99" s="1">
+        <v>1130.9349999999999</v>
+      </c>
+      <c r="C99" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D99" s="1">
+        <v>-2.0499999999999998</v>
+      </c>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
+      <c r="A100" s="1">
+        <v>825.27200000000005</v>
+      </c>
+      <c r="B100" s="1">
+        <v>1034.662</v>
+      </c>
+      <c r="C100" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D100" s="1">
+        <v>-0.05</v>
+      </c>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
+      <c r="A101" s="1">
+        <v>825.471</v>
+      </c>
+      <c r="B101" s="1">
+        <v>937.12900000000002</v>
+      </c>
+      <c r="C101" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D101" s="1">
+        <v>1.95</v>
+      </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
+      <c r="A102" s="1">
+        <v>826.01800000000003</v>
+      </c>
+      <c r="B102" s="1">
+        <v>839.89499999999998</v>
+      </c>
+      <c r="C102" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D102" s="1">
+        <v>3.95</v>
+      </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
+      <c r="A103" s="1">
+        <v>827.74900000000002</v>
+      </c>
+      <c r="B103" s="1">
+        <v>742.09400000000005</v>
+      </c>
+      <c r="C103" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D103" s="1">
+        <v>5.92</v>
+      </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
+      <c r="A104" s="1">
+        <v>829.74400000000003</v>
+      </c>
+      <c r="B104" s="1">
+        <v>642.82299999999998</v>
+      </c>
+      <c r="C104" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D104" s="1">
+        <v>7.95</v>
+      </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
+      <c r="A105" s="1">
+        <v>832.24599999999998</v>
+      </c>
+      <c r="B105" s="1">
+        <v>543.90099999999995</v>
+      </c>
+      <c r="C105" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D105" s="1">
+        <v>9.9700000000000006</v>
+      </c>
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
+      <c r="A106" s="1">
+        <v>835.49900000000002</v>
+      </c>
+      <c r="B106" s="1">
+        <v>444.233</v>
+      </c>
+      <c r="C106" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D106" s="1">
+        <v>12</v>
+      </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
+      <c r="A107" s="1">
+        <v>839.11300000000006</v>
+      </c>
+      <c r="B107" s="1">
+        <v>345.55099999999999</v>
+      </c>
+      <c r="C107" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D107" s="1">
+        <v>14</v>
+      </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
+      <c r="A108" s="1">
+        <v>843.38099999999997</v>
+      </c>
+      <c r="B108" s="1">
+        <v>244.86500000000001</v>
+      </c>
+      <c r="C108" s="1">
+        <v>2999.5</v>
+      </c>
+      <c r="D108" s="1">
+        <v>15.97</v>
+      </c>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>